<commit_message>
remove empty rows at end of file
</commit_message>
<xml_diff>
--- a/source_data/40_data.xlsx
+++ b/source_data/40_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingyan.hu\Downloads\Step2_MinSetStaticCopy_reformat&amp;upload\DataTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonzalezmorales\projects\gender_data_portal\source_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81A8F66-4BA1-42BB-A976-9FD5538B9901}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B337CFC-29A0-430C-A42C-1C349A19E580}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="indicator_40_data " sheetId="1" r:id="rId1"/>
@@ -1931,11 +1931,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA1747"/>
+  <dimension ref="A1:AA1069"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1:E1"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1052" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S1064" sqref="S1064"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -84088,2040 +84088,6 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="1070" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="F1070" s="1"/>
-    </row>
-    <row r="1071" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="F1071" s="1"/>
-    </row>
-    <row r="1072" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="F1072" s="1"/>
-    </row>
-    <row r="1073" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1073" s="1"/>
-    </row>
-    <row r="1074" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1074" s="1"/>
-    </row>
-    <row r="1075" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1075" s="1"/>
-    </row>
-    <row r="1076" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1076" s="1"/>
-    </row>
-    <row r="1077" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1077" s="1"/>
-    </row>
-    <row r="1078" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1078" s="1"/>
-    </row>
-    <row r="1079" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1079" s="1"/>
-    </row>
-    <row r="1080" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1080" s="1"/>
-    </row>
-    <row r="1081" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1081" s="1"/>
-    </row>
-    <row r="1082" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1082" s="1"/>
-    </row>
-    <row r="1083" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1083" s="1"/>
-    </row>
-    <row r="1084" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1084" s="1"/>
-    </row>
-    <row r="1085" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1085" s="1"/>
-    </row>
-    <row r="1086" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1086" s="1"/>
-    </row>
-    <row r="1087" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1087" s="1"/>
-    </row>
-    <row r="1088" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1088" s="1"/>
-    </row>
-    <row r="1089" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1089" s="1"/>
-    </row>
-    <row r="1090" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1090" s="1"/>
-    </row>
-    <row r="1091" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1091" s="1"/>
-    </row>
-    <row r="1092" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1092" s="1"/>
-    </row>
-    <row r="1093" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1093" s="1"/>
-    </row>
-    <row r="1094" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1094" s="1"/>
-    </row>
-    <row r="1095" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1095" s="1"/>
-    </row>
-    <row r="1096" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1096" s="1"/>
-    </row>
-    <row r="1097" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1097" s="1"/>
-    </row>
-    <row r="1098" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1098" s="1"/>
-    </row>
-    <row r="1099" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1099" s="1"/>
-    </row>
-    <row r="1100" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1100" s="1"/>
-    </row>
-    <row r="1101" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1101" s="1"/>
-    </row>
-    <row r="1102" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1102" s="1"/>
-    </row>
-    <row r="1103" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1103" s="1"/>
-    </row>
-    <row r="1104" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1104" s="1"/>
-    </row>
-    <row r="1105" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1105" s="1"/>
-    </row>
-    <row r="1106" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1106" s="1"/>
-    </row>
-    <row r="1107" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1107" s="1"/>
-    </row>
-    <row r="1108" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1108" s="1"/>
-    </row>
-    <row r="1109" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1109" s="1"/>
-    </row>
-    <row r="1110" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1110" s="1"/>
-    </row>
-    <row r="1111" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1111" s="1"/>
-    </row>
-    <row r="1112" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1112" s="1"/>
-    </row>
-    <row r="1113" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1113" s="1"/>
-    </row>
-    <row r="1114" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1114" s="1"/>
-    </row>
-    <row r="1115" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1115" s="1"/>
-    </row>
-    <row r="1116" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1116" s="1"/>
-    </row>
-    <row r="1117" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1117" s="1"/>
-    </row>
-    <row r="1118" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1118" s="1"/>
-    </row>
-    <row r="1119" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1119" s="1"/>
-    </row>
-    <row r="1120" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1120" s="1"/>
-    </row>
-    <row r="1121" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1121" s="1"/>
-    </row>
-    <row r="1122" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1122" s="1"/>
-    </row>
-    <row r="1123" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1123" s="1"/>
-    </row>
-    <row r="1124" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1124" s="1"/>
-    </row>
-    <row r="1125" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1125" s="1"/>
-    </row>
-    <row r="1126" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1126" s="1"/>
-    </row>
-    <row r="1127" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1127" s="1"/>
-    </row>
-    <row r="1128" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1128" s="1"/>
-    </row>
-    <row r="1129" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1129" s="1"/>
-    </row>
-    <row r="1130" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1130" s="1"/>
-    </row>
-    <row r="1131" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1131" s="1"/>
-    </row>
-    <row r="1132" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1132" s="1"/>
-    </row>
-    <row r="1133" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1133" s="1"/>
-    </row>
-    <row r="1134" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1134" s="1"/>
-    </row>
-    <row r="1135" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1135" s="1"/>
-    </row>
-    <row r="1136" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1136" s="1"/>
-    </row>
-    <row r="1137" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1137" s="1"/>
-    </row>
-    <row r="1138" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1138" s="1"/>
-    </row>
-    <row r="1139" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1139" s="1"/>
-    </row>
-    <row r="1140" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1140" s="1"/>
-    </row>
-    <row r="1141" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1141" s="1"/>
-    </row>
-    <row r="1142" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1142" s="1"/>
-    </row>
-    <row r="1143" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1143" s="1"/>
-    </row>
-    <row r="1144" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1144" s="1"/>
-    </row>
-    <row r="1145" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1145" s="1"/>
-    </row>
-    <row r="1146" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1146" s="1"/>
-    </row>
-    <row r="1147" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1147" s="1"/>
-    </row>
-    <row r="1148" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1148" s="1"/>
-    </row>
-    <row r="1149" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1149" s="1"/>
-    </row>
-    <row r="1150" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1150" s="1"/>
-    </row>
-    <row r="1151" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1151" s="1"/>
-    </row>
-    <row r="1152" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1152" s="1"/>
-    </row>
-    <row r="1153" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1153" s="1"/>
-    </row>
-    <row r="1154" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1154" s="1"/>
-    </row>
-    <row r="1155" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1155" s="1"/>
-    </row>
-    <row r="1156" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1156" s="1"/>
-    </row>
-    <row r="1157" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1157" s="1"/>
-    </row>
-    <row r="1158" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1158" s="1"/>
-    </row>
-    <row r="1159" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1159" s="1"/>
-    </row>
-    <row r="1160" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1160" s="1"/>
-    </row>
-    <row r="1161" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1161" s="1"/>
-    </row>
-    <row r="1162" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1162" s="1"/>
-    </row>
-    <row r="1163" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1163" s="1"/>
-    </row>
-    <row r="1164" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1164" s="1"/>
-    </row>
-    <row r="1165" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1165" s="1"/>
-    </row>
-    <row r="1166" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1166" s="1"/>
-    </row>
-    <row r="1167" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1167" s="1"/>
-    </row>
-    <row r="1168" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1168" s="1"/>
-    </row>
-    <row r="1169" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1169" s="1"/>
-    </row>
-    <row r="1170" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1170" s="1"/>
-    </row>
-    <row r="1171" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1171" s="1"/>
-    </row>
-    <row r="1172" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1172" s="1"/>
-    </row>
-    <row r="1173" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1173" s="1"/>
-    </row>
-    <row r="1174" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1174" s="1"/>
-    </row>
-    <row r="1175" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1175" s="1"/>
-    </row>
-    <row r="1176" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1176" s="1"/>
-    </row>
-    <row r="1177" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1177" s="1"/>
-    </row>
-    <row r="1178" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1178" s="1"/>
-    </row>
-    <row r="1179" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1179" s="1"/>
-    </row>
-    <row r="1180" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1180" s="1"/>
-    </row>
-    <row r="1181" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1181" s="1"/>
-    </row>
-    <row r="1182" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1182" s="1"/>
-    </row>
-    <row r="1183" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1183" s="1"/>
-    </row>
-    <row r="1184" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1184" s="1"/>
-    </row>
-    <row r="1185" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1185" s="1"/>
-    </row>
-    <row r="1186" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1186" s="1"/>
-    </row>
-    <row r="1187" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1187" s="1"/>
-    </row>
-    <row r="1188" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1188" s="1"/>
-    </row>
-    <row r="1189" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1189" s="1"/>
-    </row>
-    <row r="1190" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1190" s="1"/>
-    </row>
-    <row r="1191" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1191" s="1"/>
-    </row>
-    <row r="1192" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1192" s="1"/>
-    </row>
-    <row r="1193" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1193" s="1"/>
-    </row>
-    <row r="1194" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1194" s="1"/>
-    </row>
-    <row r="1195" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1195" s="1"/>
-    </row>
-    <row r="1196" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1196" s="1"/>
-    </row>
-    <row r="1197" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1197" s="1"/>
-    </row>
-    <row r="1198" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1198" s="1"/>
-    </row>
-    <row r="1199" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1199" s="1"/>
-    </row>
-    <row r="1200" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1200" s="1"/>
-    </row>
-    <row r="1201" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1201" s="1"/>
-    </row>
-    <row r="1202" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1202" s="1"/>
-    </row>
-    <row r="1203" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1203" s="1"/>
-    </row>
-    <row r="1204" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1204" s="1"/>
-    </row>
-    <row r="1205" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1205" s="1"/>
-    </row>
-    <row r="1206" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1206" s="1"/>
-    </row>
-    <row r="1207" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1207" s="1"/>
-    </row>
-    <row r="1208" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1208" s="1"/>
-    </row>
-    <row r="1209" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1209" s="1"/>
-    </row>
-    <row r="1210" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1210" s="1"/>
-    </row>
-    <row r="1211" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1211" s="1"/>
-    </row>
-    <row r="1212" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1212" s="1"/>
-    </row>
-    <row r="1213" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1213" s="1"/>
-    </row>
-    <row r="1214" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1214" s="1"/>
-    </row>
-    <row r="1215" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1215" s="1"/>
-    </row>
-    <row r="1216" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1216" s="1"/>
-    </row>
-    <row r="1217" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1217" s="1"/>
-    </row>
-    <row r="1218" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1218" s="1"/>
-    </row>
-    <row r="1219" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1219" s="1"/>
-    </row>
-    <row r="1220" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1220" s="1"/>
-    </row>
-    <row r="1221" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1221" s="1"/>
-    </row>
-    <row r="1222" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1222" s="1"/>
-    </row>
-    <row r="1223" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1223" s="1"/>
-    </row>
-    <row r="1224" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1224" s="1"/>
-    </row>
-    <row r="1225" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1225" s="1"/>
-    </row>
-    <row r="1226" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1226" s="1"/>
-    </row>
-    <row r="1227" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1227" s="1"/>
-    </row>
-    <row r="1228" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1228" s="1"/>
-    </row>
-    <row r="1229" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1229" s="1"/>
-    </row>
-    <row r="1230" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1230" s="1"/>
-    </row>
-    <row r="1231" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1231" s="1"/>
-    </row>
-    <row r="1232" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1232" s="1"/>
-    </row>
-    <row r="1233" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1233" s="1"/>
-    </row>
-    <row r="1234" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1234" s="1"/>
-    </row>
-    <row r="1235" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1235" s="1"/>
-    </row>
-    <row r="1236" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1236" s="1"/>
-    </row>
-    <row r="1237" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1237" s="1"/>
-    </row>
-    <row r="1238" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1238" s="1"/>
-    </row>
-    <row r="1239" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1239" s="1"/>
-    </row>
-    <row r="1240" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1240" s="1"/>
-    </row>
-    <row r="1241" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1241" s="1"/>
-    </row>
-    <row r="1242" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1242" s="1"/>
-    </row>
-    <row r="1243" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1243" s="1"/>
-    </row>
-    <row r="1244" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1244" s="1"/>
-    </row>
-    <row r="1245" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1245" s="1"/>
-    </row>
-    <row r="1246" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1246" s="1"/>
-    </row>
-    <row r="1247" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1247" s="1"/>
-    </row>
-    <row r="1248" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1248" s="1"/>
-    </row>
-    <row r="1249" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1249" s="1"/>
-    </row>
-    <row r="1250" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1250" s="1"/>
-    </row>
-    <row r="1251" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1251" s="1"/>
-    </row>
-    <row r="1252" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1252" s="1"/>
-    </row>
-    <row r="1253" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1253" s="1"/>
-    </row>
-    <row r="1254" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1254" s="1"/>
-    </row>
-    <row r="1255" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1255" s="1"/>
-    </row>
-    <row r="1256" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1256" s="1"/>
-    </row>
-    <row r="1257" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1257" s="1"/>
-    </row>
-    <row r="1258" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1258" s="1"/>
-    </row>
-    <row r="1259" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1259" s="1"/>
-    </row>
-    <row r="1260" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1260" s="1"/>
-    </row>
-    <row r="1261" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1261" s="1"/>
-    </row>
-    <row r="1262" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1262" s="1"/>
-    </row>
-    <row r="1263" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1263" s="1"/>
-    </row>
-    <row r="1264" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1264" s="1"/>
-    </row>
-    <row r="1265" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1265" s="1"/>
-    </row>
-    <row r="1266" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1266" s="1"/>
-    </row>
-    <row r="1267" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1267" s="1"/>
-    </row>
-    <row r="1268" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1268" s="1"/>
-    </row>
-    <row r="1269" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1269" s="1"/>
-    </row>
-    <row r="1270" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1270" s="1"/>
-    </row>
-    <row r="1271" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1271" s="1"/>
-    </row>
-    <row r="1272" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1272" s="1"/>
-    </row>
-    <row r="1273" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1273" s="1"/>
-    </row>
-    <row r="1274" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1274" s="1"/>
-    </row>
-    <row r="1275" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1275" s="1"/>
-    </row>
-    <row r="1276" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1276" s="1"/>
-    </row>
-    <row r="1277" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1277" s="1"/>
-    </row>
-    <row r="1278" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1278" s="1"/>
-    </row>
-    <row r="1279" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1279" s="1"/>
-    </row>
-    <row r="1280" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1280" s="1"/>
-    </row>
-    <row r="1281" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1281" s="1"/>
-    </row>
-    <row r="1282" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1282" s="1"/>
-    </row>
-    <row r="1283" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1283" s="1"/>
-    </row>
-    <row r="1284" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1284" s="1"/>
-    </row>
-    <row r="1285" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1285" s="1"/>
-    </row>
-    <row r="1286" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1286" s="1"/>
-    </row>
-    <row r="1287" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1287" s="1"/>
-    </row>
-    <row r="1288" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1288" s="1"/>
-    </row>
-    <row r="1289" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1289" s="1"/>
-    </row>
-    <row r="1290" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1290" s="1"/>
-    </row>
-    <row r="1291" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1291" s="1"/>
-    </row>
-    <row r="1292" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1292" s="1"/>
-    </row>
-    <row r="1293" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1293" s="1"/>
-    </row>
-    <row r="1294" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1294" s="1"/>
-    </row>
-    <row r="1295" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1295" s="1"/>
-    </row>
-    <row r="1296" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1296" s="1"/>
-    </row>
-    <row r="1297" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1297" s="1"/>
-    </row>
-    <row r="1298" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1298" s="1"/>
-    </row>
-    <row r="1299" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1299" s="1"/>
-    </row>
-    <row r="1300" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1300" s="1"/>
-    </row>
-    <row r="1301" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1301" s="1"/>
-    </row>
-    <row r="1302" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1302" s="1"/>
-    </row>
-    <row r="1303" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1303" s="1"/>
-    </row>
-    <row r="1304" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1304" s="1"/>
-    </row>
-    <row r="1305" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1305" s="1"/>
-    </row>
-    <row r="1306" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1306" s="1"/>
-    </row>
-    <row r="1307" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1307" s="1"/>
-    </row>
-    <row r="1308" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1308" s="1"/>
-    </row>
-    <row r="1309" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1309" s="1"/>
-    </row>
-    <row r="1310" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1310" s="1"/>
-    </row>
-    <row r="1311" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1311" s="1"/>
-    </row>
-    <row r="1312" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1312" s="1"/>
-    </row>
-    <row r="1313" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1313" s="1"/>
-    </row>
-    <row r="1314" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1314" s="1"/>
-    </row>
-    <row r="1315" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1315" s="1"/>
-    </row>
-    <row r="1316" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1316" s="1"/>
-    </row>
-    <row r="1317" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1317" s="1"/>
-    </row>
-    <row r="1318" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1318" s="1"/>
-    </row>
-    <row r="1319" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1319" s="1"/>
-    </row>
-    <row r="1320" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1320" s="1"/>
-    </row>
-    <row r="1321" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1321" s="1"/>
-    </row>
-    <row r="1322" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1322" s="1"/>
-    </row>
-    <row r="1323" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1323" s="1"/>
-    </row>
-    <row r="1324" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1324" s="1"/>
-    </row>
-    <row r="1325" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1325" s="1"/>
-    </row>
-    <row r="1326" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1326" s="1"/>
-    </row>
-    <row r="1327" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1327" s="1"/>
-    </row>
-    <row r="1328" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1328" s="1"/>
-    </row>
-    <row r="1329" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1329" s="1"/>
-    </row>
-    <row r="1330" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1330" s="1"/>
-    </row>
-    <row r="1331" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1331" s="1"/>
-    </row>
-    <row r="1332" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1332" s="1"/>
-    </row>
-    <row r="1333" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1333" s="1"/>
-    </row>
-    <row r="1334" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1334" s="1"/>
-    </row>
-    <row r="1335" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1335" s="1"/>
-    </row>
-    <row r="1336" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1336" s="1"/>
-    </row>
-    <row r="1337" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1337" s="1"/>
-    </row>
-    <row r="1338" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1338" s="1"/>
-    </row>
-    <row r="1339" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1339" s="1"/>
-    </row>
-    <row r="1340" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1340" s="1"/>
-    </row>
-    <row r="1341" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1341" s="1"/>
-    </row>
-    <row r="1342" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1342" s="1"/>
-    </row>
-    <row r="1343" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1343" s="1"/>
-    </row>
-    <row r="1344" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1344" s="1"/>
-    </row>
-    <row r="1345" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1345" s="1"/>
-    </row>
-    <row r="1346" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1346" s="1"/>
-    </row>
-    <row r="1347" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1347" s="1"/>
-    </row>
-    <row r="1348" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1348" s="1"/>
-    </row>
-    <row r="1349" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1349" s="1"/>
-    </row>
-    <row r="1350" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1350" s="1"/>
-    </row>
-    <row r="1351" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1351" s="1"/>
-    </row>
-    <row r="1352" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1352" s="1"/>
-    </row>
-    <row r="1353" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1353" s="1"/>
-    </row>
-    <row r="1354" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1354" s="1"/>
-    </row>
-    <row r="1355" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1355" s="1"/>
-    </row>
-    <row r="1356" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1356" s="1"/>
-    </row>
-    <row r="1357" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1357" s="1"/>
-    </row>
-    <row r="1358" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1358" s="1"/>
-    </row>
-    <row r="1359" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1359" s="1"/>
-    </row>
-    <row r="1360" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1360" s="1"/>
-    </row>
-    <row r="1361" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1361" s="1"/>
-    </row>
-    <row r="1362" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1362" s="1"/>
-    </row>
-    <row r="1363" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1363" s="1"/>
-    </row>
-    <row r="1364" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1364" s="1"/>
-    </row>
-    <row r="1365" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1365" s="1"/>
-    </row>
-    <row r="1366" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1366" s="1"/>
-    </row>
-    <row r="1367" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1367" s="1"/>
-    </row>
-    <row r="1368" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1368" s="1"/>
-    </row>
-    <row r="1369" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1369" s="1"/>
-    </row>
-    <row r="1370" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1370" s="1"/>
-    </row>
-    <row r="1371" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1371" s="1"/>
-    </row>
-    <row r="1372" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1372" s="1"/>
-    </row>
-    <row r="1373" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1373" s="1"/>
-    </row>
-    <row r="1374" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1374" s="1"/>
-    </row>
-    <row r="1375" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1375" s="1"/>
-    </row>
-    <row r="1376" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1376" s="1"/>
-    </row>
-    <row r="1377" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1377" s="1"/>
-    </row>
-    <row r="1378" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1378" s="1"/>
-    </row>
-    <row r="1379" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1379" s="1"/>
-    </row>
-    <row r="1380" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1380" s="1"/>
-    </row>
-    <row r="1381" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1381" s="1"/>
-    </row>
-    <row r="1382" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1382" s="1"/>
-    </row>
-    <row r="1383" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1383" s="1"/>
-    </row>
-    <row r="1384" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1384" s="1"/>
-    </row>
-    <row r="1385" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1385" s="1"/>
-    </row>
-    <row r="1386" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1386" s="1"/>
-    </row>
-    <row r="1387" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1387" s="1"/>
-    </row>
-    <row r="1388" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1388" s="1"/>
-    </row>
-    <row r="1389" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1389" s="1"/>
-    </row>
-    <row r="1390" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1390" s="1"/>
-    </row>
-    <row r="1391" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1391" s="1"/>
-    </row>
-    <row r="1392" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1392" s="1"/>
-    </row>
-    <row r="1393" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1393" s="1"/>
-    </row>
-    <row r="1394" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1394" s="1"/>
-    </row>
-    <row r="1395" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1395" s="1"/>
-    </row>
-    <row r="1396" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1396" s="1"/>
-    </row>
-    <row r="1397" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1397" s="1"/>
-    </row>
-    <row r="1398" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1398" s="1"/>
-    </row>
-    <row r="1399" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1399" s="1"/>
-    </row>
-    <row r="1400" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1400" s="1"/>
-    </row>
-    <row r="1401" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1401" s="1"/>
-    </row>
-    <row r="1402" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1402" s="1"/>
-    </row>
-    <row r="1403" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1403" s="1"/>
-    </row>
-    <row r="1404" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1404" s="1"/>
-    </row>
-    <row r="1405" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1405" s="1"/>
-    </row>
-    <row r="1406" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1406" s="1"/>
-    </row>
-    <row r="1407" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1407" s="1"/>
-    </row>
-    <row r="1408" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1408" s="1"/>
-    </row>
-    <row r="1409" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1409" s="1"/>
-    </row>
-    <row r="1410" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1410" s="1"/>
-    </row>
-    <row r="1411" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1411" s="1"/>
-    </row>
-    <row r="1412" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1412" s="1"/>
-    </row>
-    <row r="1413" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1413" s="1"/>
-    </row>
-    <row r="1414" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1414" s="1"/>
-    </row>
-    <row r="1415" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1415" s="1"/>
-    </row>
-    <row r="1416" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1416" s="1"/>
-    </row>
-    <row r="1417" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1417" s="1"/>
-    </row>
-    <row r="1418" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1418" s="1"/>
-    </row>
-    <row r="1419" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1419" s="1"/>
-    </row>
-    <row r="1420" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1420" s="1"/>
-    </row>
-    <row r="1421" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1421" s="1"/>
-    </row>
-    <row r="1422" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1422" s="1"/>
-    </row>
-    <row r="1423" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1423" s="1"/>
-    </row>
-    <row r="1424" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1424" s="1"/>
-    </row>
-    <row r="1425" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1425" s="1"/>
-    </row>
-    <row r="1426" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1426" s="1"/>
-    </row>
-    <row r="1427" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1427" s="1"/>
-    </row>
-    <row r="1428" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1428" s="1"/>
-    </row>
-    <row r="1429" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1429" s="1"/>
-    </row>
-    <row r="1430" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1430" s="1"/>
-    </row>
-    <row r="1431" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1431" s="1"/>
-    </row>
-    <row r="1432" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1432" s="1"/>
-    </row>
-    <row r="1433" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1433" s="1"/>
-    </row>
-    <row r="1434" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1434" s="1"/>
-    </row>
-    <row r="1435" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1435" s="1"/>
-    </row>
-    <row r="1436" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1436" s="1"/>
-    </row>
-    <row r="1437" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1437" s="1"/>
-    </row>
-    <row r="1438" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1438" s="1"/>
-    </row>
-    <row r="1439" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1439" s="1"/>
-    </row>
-    <row r="1440" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1440" s="1"/>
-    </row>
-    <row r="1441" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1441" s="1"/>
-    </row>
-    <row r="1442" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1442" s="1"/>
-    </row>
-    <row r="1443" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1443" s="1"/>
-    </row>
-    <row r="1444" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1444" s="1"/>
-    </row>
-    <row r="1445" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1445" s="1"/>
-    </row>
-    <row r="1446" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1446" s="1"/>
-    </row>
-    <row r="1447" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1447" s="1"/>
-    </row>
-    <row r="1448" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1448" s="1"/>
-    </row>
-    <row r="1449" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1449" s="1"/>
-    </row>
-    <row r="1450" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1450" s="1"/>
-    </row>
-    <row r="1451" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1451" s="1"/>
-    </row>
-    <row r="1452" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1452" s="1"/>
-    </row>
-    <row r="1453" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1453" s="1"/>
-    </row>
-    <row r="1454" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1454" s="1"/>
-    </row>
-    <row r="1455" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1455" s="1"/>
-    </row>
-    <row r="1456" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1456" s="1"/>
-    </row>
-    <row r="1457" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1457" s="1"/>
-    </row>
-    <row r="1458" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1458" s="1"/>
-    </row>
-    <row r="1459" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1459" s="1"/>
-    </row>
-    <row r="1460" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1460" s="1"/>
-    </row>
-    <row r="1461" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1461" s="1"/>
-    </row>
-    <row r="1462" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1462" s="1"/>
-    </row>
-    <row r="1463" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1463" s="1"/>
-    </row>
-    <row r="1464" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1464" s="1"/>
-    </row>
-    <row r="1465" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1465" s="1"/>
-    </row>
-    <row r="1466" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1466" s="1"/>
-    </row>
-    <row r="1467" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1467" s="1"/>
-    </row>
-    <row r="1468" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1468" s="1"/>
-    </row>
-    <row r="1469" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1469" s="1"/>
-    </row>
-    <row r="1470" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1470" s="1"/>
-    </row>
-    <row r="1471" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1471" s="1"/>
-    </row>
-    <row r="1472" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1472" s="1"/>
-    </row>
-    <row r="1473" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1473" s="1"/>
-    </row>
-    <row r="1474" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1474" s="1"/>
-    </row>
-    <row r="1475" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1475" s="1"/>
-    </row>
-    <row r="1476" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1476" s="1"/>
-    </row>
-    <row r="1477" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1477" s="1"/>
-    </row>
-    <row r="1478" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1478" s="1"/>
-    </row>
-    <row r="1479" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1479" s="1"/>
-    </row>
-    <row r="1480" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1480" s="1"/>
-    </row>
-    <row r="1481" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1481" s="1"/>
-    </row>
-    <row r="1482" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1482" s="1"/>
-    </row>
-    <row r="1483" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1483" s="1"/>
-    </row>
-    <row r="1484" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1484" s="1"/>
-    </row>
-    <row r="1485" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1485" s="1"/>
-    </row>
-    <row r="1486" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1486" s="1"/>
-    </row>
-    <row r="1487" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1487" s="1"/>
-    </row>
-    <row r="1488" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1488" s="1"/>
-    </row>
-    <row r="1489" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1489" s="1"/>
-    </row>
-    <row r="1490" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1490" s="1"/>
-    </row>
-    <row r="1491" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1491" s="1"/>
-    </row>
-    <row r="1492" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1492" s="1"/>
-    </row>
-    <row r="1493" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1493" s="1"/>
-    </row>
-    <row r="1494" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1494" s="1"/>
-    </row>
-    <row r="1495" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1495" s="1"/>
-    </row>
-    <row r="1496" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1496" s="1"/>
-    </row>
-    <row r="1497" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1497" s="1"/>
-    </row>
-    <row r="1498" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1498" s="1"/>
-    </row>
-    <row r="1499" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1499" s="1"/>
-    </row>
-    <row r="1500" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1500" s="1"/>
-    </row>
-    <row r="1501" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1501" s="1"/>
-    </row>
-    <row r="1502" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1502" s="1"/>
-    </row>
-    <row r="1503" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1503" s="1"/>
-    </row>
-    <row r="1504" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1504" s="1"/>
-    </row>
-    <row r="1505" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1505" s="1"/>
-    </row>
-    <row r="1506" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1506" s="1"/>
-    </row>
-    <row r="1507" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1507" s="1"/>
-    </row>
-    <row r="1508" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1508" s="1"/>
-    </row>
-    <row r="1509" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1509" s="1"/>
-    </row>
-    <row r="1510" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1510" s="1"/>
-    </row>
-    <row r="1511" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1511" s="1"/>
-    </row>
-    <row r="1512" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1512" s="1"/>
-    </row>
-    <row r="1513" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1513" s="1"/>
-    </row>
-    <row r="1514" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1514" s="1"/>
-    </row>
-    <row r="1515" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1515" s="1"/>
-    </row>
-    <row r="1516" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1516" s="1"/>
-    </row>
-    <row r="1517" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1517" s="1"/>
-    </row>
-    <row r="1518" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1518" s="1"/>
-    </row>
-    <row r="1519" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1519" s="1"/>
-    </row>
-    <row r="1520" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1520" s="1"/>
-    </row>
-    <row r="1521" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1521" s="1"/>
-    </row>
-    <row r="1522" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1522" s="1"/>
-    </row>
-    <row r="1523" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1523" s="1"/>
-    </row>
-    <row r="1524" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1524" s="1"/>
-    </row>
-    <row r="1525" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1525" s="1"/>
-    </row>
-    <row r="1526" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1526" s="1"/>
-    </row>
-    <row r="1527" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1527" s="1"/>
-    </row>
-    <row r="1528" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1528" s="1"/>
-    </row>
-    <row r="1529" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1529" s="1"/>
-    </row>
-    <row r="1530" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1530" s="1"/>
-    </row>
-    <row r="1531" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1531" s="1"/>
-    </row>
-    <row r="1532" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1532" s="1"/>
-    </row>
-    <row r="1533" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1533" s="1"/>
-    </row>
-    <row r="1534" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1534" s="1"/>
-    </row>
-    <row r="1535" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1535" s="1"/>
-    </row>
-    <row r="1536" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1536" s="1"/>
-    </row>
-    <row r="1537" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1537" s="1"/>
-    </row>
-    <row r="1538" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1538" s="1"/>
-    </row>
-    <row r="1539" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1539" s="1"/>
-    </row>
-    <row r="1540" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1540" s="1"/>
-    </row>
-    <row r="1541" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1541" s="1"/>
-    </row>
-    <row r="1542" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1542" s="1"/>
-    </row>
-    <row r="1543" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1543" s="1"/>
-    </row>
-    <row r="1544" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1544" s="1"/>
-    </row>
-    <row r="1545" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1545" s="1"/>
-    </row>
-    <row r="1546" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1546" s="1"/>
-    </row>
-    <row r="1547" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1547" s="1"/>
-    </row>
-    <row r="1548" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1548" s="1"/>
-    </row>
-    <row r="1549" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1549" s="1"/>
-    </row>
-    <row r="1550" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1550" s="1"/>
-    </row>
-    <row r="1551" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1551" s="1"/>
-    </row>
-    <row r="1552" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1552" s="1"/>
-    </row>
-    <row r="1553" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1553" s="1"/>
-    </row>
-    <row r="1554" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1554" s="1"/>
-    </row>
-    <row r="1555" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1555" s="1"/>
-    </row>
-    <row r="1556" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1556" s="1"/>
-    </row>
-    <row r="1557" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1557" s="1"/>
-    </row>
-    <row r="1558" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1558" s="1"/>
-    </row>
-    <row r="1559" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1559" s="1"/>
-    </row>
-    <row r="1560" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1560" s="1"/>
-    </row>
-    <row r="1561" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1561" s="1"/>
-    </row>
-    <row r="1562" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1562" s="1"/>
-    </row>
-    <row r="1563" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1563" s="1"/>
-    </row>
-    <row r="1564" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1564" s="1"/>
-    </row>
-    <row r="1565" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1565" s="1"/>
-    </row>
-    <row r="1566" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1566" s="1"/>
-    </row>
-    <row r="1567" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1567" s="1"/>
-    </row>
-    <row r="1568" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1568" s="1"/>
-    </row>
-    <row r="1569" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1569" s="1"/>
-    </row>
-    <row r="1570" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1570" s="1"/>
-    </row>
-    <row r="1571" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1571" s="1"/>
-    </row>
-    <row r="1572" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1572" s="1"/>
-    </row>
-    <row r="1573" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1573" s="1"/>
-    </row>
-    <row r="1574" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1574" s="1"/>
-    </row>
-    <row r="1575" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1575" s="1"/>
-    </row>
-    <row r="1576" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1576" s="1"/>
-    </row>
-    <row r="1577" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1577" s="1"/>
-    </row>
-    <row r="1578" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1578" s="1"/>
-    </row>
-    <row r="1579" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1579" s="1"/>
-    </row>
-    <row r="1580" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1580" s="1"/>
-    </row>
-    <row r="1581" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1581" s="1"/>
-    </row>
-    <row r="1582" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1582" s="1"/>
-    </row>
-    <row r="1583" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1583" s="1"/>
-    </row>
-    <row r="1584" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1584" s="1"/>
-    </row>
-    <row r="1585" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1585" s="1"/>
-    </row>
-    <row r="1586" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1586" s="1"/>
-    </row>
-    <row r="1587" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1587" s="1"/>
-    </row>
-    <row r="1588" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1588" s="1"/>
-    </row>
-    <row r="1589" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1589" s="1"/>
-    </row>
-    <row r="1590" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1590" s="1"/>
-    </row>
-    <row r="1591" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1591" s="1"/>
-    </row>
-    <row r="1592" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1592" s="1"/>
-    </row>
-    <row r="1593" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1593" s="1"/>
-    </row>
-    <row r="1594" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1594" s="1"/>
-    </row>
-    <row r="1595" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1595" s="1"/>
-    </row>
-    <row r="1596" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1596" s="1"/>
-    </row>
-    <row r="1597" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1597" s="1"/>
-    </row>
-    <row r="1598" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1598" s="1"/>
-    </row>
-    <row r="1599" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1599" s="1"/>
-    </row>
-    <row r="1600" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1600" s="1"/>
-    </row>
-    <row r="1601" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1601" s="1"/>
-    </row>
-    <row r="1602" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1602" s="1"/>
-    </row>
-    <row r="1603" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1603" s="1"/>
-    </row>
-    <row r="1604" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1604" s="1"/>
-    </row>
-    <row r="1605" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1605" s="1"/>
-    </row>
-    <row r="1606" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1606" s="1"/>
-    </row>
-    <row r="1607" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1607" s="1"/>
-    </row>
-    <row r="1608" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1608" s="1"/>
-    </row>
-    <row r="1609" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1609" s="1"/>
-    </row>
-    <row r="1610" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1610" s="1"/>
-    </row>
-    <row r="1611" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1611" s="1"/>
-    </row>
-    <row r="1612" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1612" s="1"/>
-    </row>
-    <row r="1613" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1613" s="1"/>
-    </row>
-    <row r="1614" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1614" s="1"/>
-    </row>
-    <row r="1615" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1615" s="1"/>
-    </row>
-    <row r="1616" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1616" s="1"/>
-    </row>
-    <row r="1617" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1617" s="1"/>
-    </row>
-    <row r="1618" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1618" s="1"/>
-    </row>
-    <row r="1619" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1619" s="1"/>
-    </row>
-    <row r="1620" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1620" s="1"/>
-    </row>
-    <row r="1621" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1621" s="1"/>
-    </row>
-    <row r="1622" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1622" s="1"/>
-    </row>
-    <row r="1623" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1623" s="1"/>
-    </row>
-    <row r="1624" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1624" s="1"/>
-    </row>
-    <row r="1625" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1625" s="1"/>
-    </row>
-    <row r="1626" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1626" s="1"/>
-    </row>
-    <row r="1627" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1627" s="1"/>
-    </row>
-    <row r="1628" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1628" s="1"/>
-    </row>
-    <row r="1629" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1629" s="1"/>
-    </row>
-    <row r="1630" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1630" s="1"/>
-    </row>
-    <row r="1631" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1631" s="1"/>
-    </row>
-    <row r="1632" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1632" s="1"/>
-    </row>
-    <row r="1633" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1633" s="1"/>
-    </row>
-    <row r="1634" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1634" s="1"/>
-    </row>
-    <row r="1635" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1635" s="1"/>
-    </row>
-    <row r="1636" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1636" s="1"/>
-    </row>
-    <row r="1637" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1637" s="1"/>
-    </row>
-    <row r="1638" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1638" s="1"/>
-    </row>
-    <row r="1639" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1639" s="1"/>
-    </row>
-    <row r="1640" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1640" s="1"/>
-    </row>
-    <row r="1641" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1641" s="1"/>
-    </row>
-    <row r="1642" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1642" s="1"/>
-    </row>
-    <row r="1643" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1643" s="1"/>
-    </row>
-    <row r="1644" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1644" s="1"/>
-    </row>
-    <row r="1645" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1645" s="1"/>
-    </row>
-    <row r="1646" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1646" s="1"/>
-    </row>
-    <row r="1647" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1647" s="1"/>
-    </row>
-    <row r="1648" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1648" s="1"/>
-    </row>
-    <row r="1649" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1649" s="1"/>
-    </row>
-    <row r="1650" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1650" s="1"/>
-    </row>
-    <row r="1651" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1651" s="1"/>
-    </row>
-    <row r="1652" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1652" s="1"/>
-    </row>
-    <row r="1653" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1653" s="1"/>
-    </row>
-    <row r="1654" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1654" s="1"/>
-    </row>
-    <row r="1655" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1655" s="1"/>
-    </row>
-    <row r="1656" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1656" s="1"/>
-    </row>
-    <row r="1657" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1657" s="1"/>
-    </row>
-    <row r="1658" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1658" s="1"/>
-    </row>
-    <row r="1659" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1659" s="1"/>
-    </row>
-    <row r="1660" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1660" s="1"/>
-    </row>
-    <row r="1661" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1661" s="1"/>
-    </row>
-    <row r="1662" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1662" s="1"/>
-    </row>
-    <row r="1663" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1663" s="1"/>
-    </row>
-    <row r="1664" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1664" s="1"/>
-    </row>
-    <row r="1665" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1665" s="1"/>
-    </row>
-    <row r="1666" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1666" s="1"/>
-    </row>
-    <row r="1667" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1667" s="1"/>
-    </row>
-    <row r="1668" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1668" s="1"/>
-    </row>
-    <row r="1669" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1669" s="1"/>
-    </row>
-    <row r="1670" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1670" s="1"/>
-    </row>
-    <row r="1671" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1671" s="1"/>
-    </row>
-    <row r="1672" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1672" s="1"/>
-    </row>
-    <row r="1673" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1673" s="1"/>
-    </row>
-    <row r="1674" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1674" s="1"/>
-    </row>
-    <row r="1675" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1675" s="1"/>
-    </row>
-    <row r="1676" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1676" s="1"/>
-    </row>
-    <row r="1677" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1677" s="1"/>
-    </row>
-    <row r="1678" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1678" s="1"/>
-    </row>
-    <row r="1679" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1679" s="1"/>
-    </row>
-    <row r="1680" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1680" s="1"/>
-    </row>
-    <row r="1681" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1681" s="1"/>
-    </row>
-    <row r="1682" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1682" s="1"/>
-    </row>
-    <row r="1683" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1683" s="1"/>
-    </row>
-    <row r="1684" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1684" s="1"/>
-    </row>
-    <row r="1685" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1685" s="1"/>
-    </row>
-    <row r="1686" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1686" s="1"/>
-    </row>
-    <row r="1687" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1687" s="1"/>
-    </row>
-    <row r="1688" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1688" s="1"/>
-    </row>
-    <row r="1689" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1689" s="1"/>
-    </row>
-    <row r="1690" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1690" s="1"/>
-    </row>
-    <row r="1691" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1691" s="1"/>
-    </row>
-    <row r="1692" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1692" s="1"/>
-    </row>
-    <row r="1693" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1693" s="1"/>
-    </row>
-    <row r="1694" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1694" s="1"/>
-    </row>
-    <row r="1695" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1695" s="1"/>
-    </row>
-    <row r="1696" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1696" s="1"/>
-    </row>
-    <row r="1697" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1697" s="1"/>
-    </row>
-    <row r="1698" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1698" s="1"/>
-    </row>
-    <row r="1699" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1699" s="1"/>
-    </row>
-    <row r="1700" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1700" s="1"/>
-    </row>
-    <row r="1701" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1701" s="1"/>
-    </row>
-    <row r="1702" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1702" s="1"/>
-    </row>
-    <row r="1703" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1703" s="1"/>
-    </row>
-    <row r="1704" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1704" s="1"/>
-    </row>
-    <row r="1705" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1705" s="1"/>
-    </row>
-    <row r="1706" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1706" s="1"/>
-    </row>
-    <row r="1707" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1707" s="1"/>
-    </row>
-    <row r="1708" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1708" s="1"/>
-    </row>
-    <row r="1709" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1709" s="1"/>
-    </row>
-    <row r="1710" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1710" s="1"/>
-    </row>
-    <row r="1711" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1711" s="1"/>
-    </row>
-    <row r="1712" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1712" s="1"/>
-    </row>
-    <row r="1713" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1713" s="1"/>
-    </row>
-    <row r="1714" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1714" s="1"/>
-    </row>
-    <row r="1715" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1715" s="1"/>
-    </row>
-    <row r="1716" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1716" s="1"/>
-    </row>
-    <row r="1717" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1717" s="1"/>
-    </row>
-    <row r="1718" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1718" s="1"/>
-    </row>
-    <row r="1719" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1719" s="1"/>
-    </row>
-    <row r="1720" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1720" s="1"/>
-    </row>
-    <row r="1721" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1721" s="1"/>
-    </row>
-    <row r="1722" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1722" s="1"/>
-    </row>
-    <row r="1723" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1723" s="1"/>
-    </row>
-    <row r="1724" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1724" s="1"/>
-    </row>
-    <row r="1725" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1725" s="1"/>
-    </row>
-    <row r="1726" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1726" s="1"/>
-    </row>
-    <row r="1727" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1727" s="1"/>
-    </row>
-    <row r="1728" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1728" s="1"/>
-    </row>
-    <row r="1729" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1729" s="1"/>
-    </row>
-    <row r="1730" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1730" s="1"/>
-    </row>
-    <row r="1731" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1731" s="1"/>
-    </row>
-    <row r="1732" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1732" s="1"/>
-    </row>
-    <row r="1733" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1733" s="1"/>
-    </row>
-    <row r="1734" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1734" s="1"/>
-    </row>
-    <row r="1735" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1735" s="1"/>
-    </row>
-    <row r="1736" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1736" s="1"/>
-    </row>
-    <row r="1737" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1737" s="1"/>
-    </row>
-    <row r="1738" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1738" s="1"/>
-    </row>
-    <row r="1739" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1739" s="1"/>
-    </row>
-    <row r="1740" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1740" s="1"/>
-    </row>
-    <row r="1741" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1741" s="1"/>
-    </row>
-    <row r="1742" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1742" s="1"/>
-    </row>
-    <row r="1743" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1743" s="1"/>
-    </row>
-    <row r="1744" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1744" s="1"/>
-    </row>
-    <row r="1745" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1745" s="1"/>
-    </row>
-    <row r="1746" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1746" s="1"/>
-    </row>
-    <row r="1747" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1747" s="1"/>
-    </row>
   </sheetData>
   <autoFilter ref="A1:AA1069" xr:uid="{5A4B1E4C-627B-4425-90F4-740ACE2C4F93}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AA269">

</xml_diff>